<commit_message>
test5:changing the layout of the clinical forms
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
   <si>
     <t>type</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Medical care</t>
-  </si>
-  <si>
-    <t>horizontal</t>
   </si>
   <si>
     <t>select_one knowledge</t>
@@ -382,7 +379,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -405,6 +402,11 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
@@ -413,7 +415,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +426,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -447,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -475,7 +483,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -485,7 +496,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -822,121 +833,103 @@
       <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="D13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
@@ -965,13 +958,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -980,10 +973,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3">
@@ -991,10 +984,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4">
@@ -1002,10 +995,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -1013,351 +1006,351 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1382,28 +1375,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>9</v>
@@ -1412,13 +1405,13 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
category:Adding the ability to dynamically select the risk category based on the total score of the level of care assessment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -24,6 +24,9 @@
     <t>label</t>
   </si>
   <si>
+    <t>relevant</t>
+  </si>
+  <si>
     <t>calculation</t>
   </si>
   <si>
@@ -39,7 +42,55 @@
     <t>Level of Care Assessment</t>
   </si>
   <si>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
     <t>field-list</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
   <si>
     <t>end group</t>
@@ -147,6 +198,12 @@
  if(selected(${communication}, 'co'), 1, 0) + if(selected(${communication}, 'temporary'), 2, 0) + if(selected(${communication}, 'limitted'), 3, 0) + if(selected(${communication}, 'xx'), 4, 0) + 
  if(selected(${employment}, 'employed'), 1, 0) + if(selected(${employment}, 'ltd_probs'), 2, 0) + if(selected(${employment}, 'unemployed'), 3, 0) + if(selected(${employment}, 'unable'), 4, 0) + 
  if(selected(${living}, 'self_managed'), 1, 0) + if(selected(${living}, 'adequate'), 2, 0) + if(selected(${living}, 'unsafe'), 3, 0) + if(selected(${living}, 'homless'), 4, 0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">category </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if((${score} &gt;= 1 and ${score} &lt;= 15), 'Limitted', if((${score} &gt;= 16  and ${score} &lt; 40 ), 'Supportive', if((${score} &gt;= 40), 'Comprehensive','')))</t>
   </si>
   <si>
     <t>note</t>
@@ -172,6 +229,12 @@
     </r>
   </si>
   <si>
+    <t>category_note</t>
+  </si>
+  <si>
+    <t>Risk Category is:${category}</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -410,11 +473,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -427,8 +491,24 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF833C0B"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF833C0B"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -450,7 +530,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +541,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
@@ -490,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -503,31 +589,33 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -537,7 +625,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -765,12 +853,12 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.71"/>
-    <col customWidth="1" min="2" max="2" width="22.43"/>
-    <col customWidth="1" min="3" max="3" width="36.14"/>
-    <col customWidth="1" min="4" max="4" width="161.86"/>
+    <col customWidth="1" min="1" max="1" width="28.63"/>
+    <col customWidth="1" min="2" max="2" width="19.63"/>
+    <col customWidth="1" min="3" max="4" width="31.63"/>
+    <col customWidth="1" min="5" max="5" width="141.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -783,28 +871,33 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -824,16 +917,23 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -853,161 +953,710 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" ht="145.5" customHeight="1">
+      <c r="A29" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="16"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" ht="145.5" customHeight="1">
-      <c r="A14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1022,405 +1671,405 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.57"/>
+    <col customWidth="1" min="1" max="1" width="19.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1436,52 +2085,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.86"/>
-    <col customWidth="1" min="2" max="2" width="24.0"/>
-    <col customWidth="1" min="6" max="6" width="17.86"/>
+    <col customWidth="1" min="1" max="1" width="22.63"/>
+    <col customWidth="1" min="2" max="2" width="21.0"/>
+    <col customWidth="1" min="6" max="6" width="15.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="16"/>
+        <v>138</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="20"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4">
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task:Add Level of care assessment task
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
     <t>type</t>
   </si>
@@ -96,6 +96,24 @@
     <t>end group</t>
   </si>
   <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient ID	</t>
+  </si>
+  <si>
+    <t>../inputs/contact/patient_id</t>
+  </si>
+  <si>
+    <t>patient_name</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name</t>
+  </si>
+  <si>
     <t>care</t>
   </si>
   <si>
@@ -181,9 +199,6 @@
   </si>
   <si>
     <t>Living situation</t>
-  </si>
-  <si>
-    <t>calculate</t>
   </si>
   <si>
     <t>score</t>
@@ -576,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -606,6 +621,12 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -1466,46 +1487,92 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4" t="s">
+      <c r="B21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="14"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
@@ -1518,7 +1585,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
@@ -1527,11 +1594,11 @@
       <c r="B23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="14"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
@@ -1544,7 +1611,7 @@
         <v>43</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="14"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
@@ -1557,7 +1624,7 @@
         <v>46</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
@@ -1570,7 +1637,7 @@
         <v>49</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="16"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
@@ -1583,7 +1650,7 @@
         <v>52</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="14"/>
+      <c r="E27" s="16"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
@@ -1596,67 +1663,93 @@
         <v>55</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" ht="145.5" customHeight="1">
-      <c r="A29" s="15" t="s">
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="16"/>
     </row>
     <row r="30">
-      <c r="A30" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="13" t="s">
+      <c r="B30" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="16" t="s">
+      <c r="C30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="D30" s="4"/>
+      <c r="E30" s="16"/>
+    </row>
+    <row r="31" ht="145.5" customHeight="1">
+      <c r="A31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="14"/>
     </row>
     <row r="32">
-      <c r="A32" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="16" t="s">
+      <c r="A32" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="14"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="4"/>
+    <row r="36">
+      <c r="A36" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1677,399 +1770,399 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2094,43 +2187,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="20"/>
+        <v>143</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="22"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4">
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
card:Implement a condition card to display the risk category depending on the total score in the level of care assessment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
   <si>
     <t>type</t>
   </si>
@@ -33,6 +33,9 @@
     <t>appearance</t>
   </si>
   <si>
+    <t>required</t>
+  </si>
+  <si>
     <t>begin group</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
   </si>
   <si>
     <t>db-object</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>string</t>
@@ -901,23 +907,26 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -942,18 +951,18 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="6"/>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -978,18 +987,18 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="6"/>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1014,13 +1023,13 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="6"/>
@@ -1048,20 +1057,22 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
       <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1084,18 +1095,18 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -1120,18 +1131,18 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -1156,18 +1167,18 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -1192,18 +1203,18 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1228,13 +1239,13 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -1262,13 +1273,13 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -1296,18 +1307,18 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1332,18 +1343,18 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1368,7 +1379,7 @@
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -1398,7 +1409,7 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>
@@ -1428,7 +1439,7 @@
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="8"/>
@@ -1458,7 +1469,7 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="8"/>
@@ -1488,17 +1499,17 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="5"/>
@@ -1524,17 +1535,17 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
@@ -1560,192 +1571,192 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="16"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="16"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="16"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="16"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="16"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="16"/>
     </row>
     <row r="31" ht="145.5" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
       <c r="E32" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="16"/>
     </row>
     <row r="34">
       <c r="A34" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="16"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
@@ -1771,7 +1782,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -1782,387 +1793,387 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2187,43 +2198,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G1" s="22"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="4">
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
care:updating the level of care assessment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="197">
   <si>
     <t>type</t>
   </si>
@@ -207,14 +207,64 @@
     <t>Living situation</t>
   </si>
   <si>
+    <t>select_one financial</t>
+  </si>
+  <si>
+    <t>financial</t>
+  </si>
+  <si>
+    <t>Financial Resources</t>
+  </si>
+  <si>
+    <t>select_one legal</t>
+  </si>
+  <si>
+    <t>legal</t>
+  </si>
+  <si>
+    <t>Legal Affiars</t>
+  </si>
+  <si>
+    <t>select_one practical</t>
+  </si>
+  <si>
+    <t>practical</t>
+  </si>
+  <si>
+    <t>Practical Assistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one activities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">activities </t>
+  </si>
+  <si>
+    <t>Self-Sustaining Activities</t>
+  </si>
+  <si>
+    <t>select_one dental</t>
+  </si>
+  <si>
+    <t>dental</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
     <t>score</t>
   </si>
   <si>
-    <t xml:space="preserve"> if(selected(${medical}, 'zero'), 1, 0) + if(selected(${medical}, 'two'), 2, 0) + if(selected(${medical}, 'five'), 3, 0) + if(selected(${medical}, 'fifty'), 4, 0) + 
+    <t xml:space="preserve">if(selected(${medical}, 'zero'), 1, 0) + if(selected(${medical}, 'two'), 2, 0) + if(selected(${medical}, 'five'), 3, 0) + if(selected(${medical}, 'fifty'), 4, 0) + 
  if(selected(${knowledge}, 'good'), 1, 0) + if(selected(${knowledge}, 'some_what'), 2, 0) + if(selected(${knowledge}, 'little'), 3, 0) + if(selected(${knowledge}, 'none'), 4, 0) + 
  if(selected(${adherence}, 'always'), 1, 0) + if(selected(${adherence}, 'usually'), 2, 0) + if(selected(${adherence}, 'rarely'), 3, 0) + if(selected(${adherence}, 'never'), 4, 0) + 
  if(selected(${mental}, 'no_history'), 1, 0) + if(selected(${mental}, 'has_access'), 2, 0) + if(selected(${mental}, 'failed_treatment'), 3, 0) + if(selected(${mental}, 'serious'), 4, 0) + 
  if(selected(${transportation}, 'consistent'), 1, 0) + if(selected(${transportation}, 'questionable'), 2, 0) + if(selected(${transportation}, 'irregular'), 3, 0) + if(selected(${transportation}, 'tr'), 4, 0) + 
+  if(selected(${financial}, 'financial_stable'), 1, 0) + if(selected(${financial}, 'financial_adequate'), 2, 0) + if(selected(${financial}, 'financial_inadequate'), 3, 0) + if(selected(${financial}, 'financial_none'), 4, 0) + 
+ if(selected(${legal}, 'none'), 1, 0) + if(selected(${legal}, 'needs_help'), 2, 0) + if(selected(${legal}, 'some_asst'), 3, 0) + if(selected(${legal}, 'full_asst'), 4, 0) + 
+ if(selected(${practical}, 'practical_inadequate'), 1, 0) + if(selected(${practical}, 'practical_some_asst'), 2, 0) + if(selected(${practical}, 'practical_limitted'), 3, 0) + if(selected(${practical}, 'practical_unable'), 4, 0) +   
+  if(selected(${activities}, 'activities_regular'), 1, 0) + if(selected(${activities}, 'activities_needs'), 2, 0) + if(selected(${activities}, 'activities_resists'), 3, 0) + if(selected(${activities}, 'activities_isolated'), 4, 0) + 
+  if(selected(${dental}, 'dental_none'), 1, 0) + if(selected(${dental}, 'dental_minor'), 2, 0) + if(selected(${dental}, 'dental_moderate'), 3, 0) + if(selected(${dental}, 'dental_major'), 4, 0) + 
  if(selected(${support}, 'reliable'), 1, 0) + if(selected(${support}, 'only'), 2, 0) + if(selected(${support}, 'su'), 3, 0) + 
  if(selected(${communication}, 'co'), 1, 0) + if(selected(${communication}, 'temporary'), 2, 0) + if(selected(${communication}, 'limitted'), 3, 0) + if(selected(${communication}, 'xx'), 4, 0) + 
  if(selected(${employment}, 'employed'), 1, 0) + if(selected(${employment}, 'ltd_probs'), 2, 0) + if(selected(${employment}, 'unemployed'), 3, 0) + if(selected(${employment}, 'unable'), 4, 0) + 
@@ -458,6 +508,99 @@
   </si>
   <si>
     <t>Homeless</t>
+  </si>
+  <si>
+    <t>financial_stable</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>financial_adequate</t>
+  </si>
+  <si>
+    <t>financial_inadequate</t>
+  </si>
+  <si>
+    <t>Inadequate</t>
+  </si>
+  <si>
+    <t>financial_none</t>
+  </si>
+  <si>
+    <t>needs_help</t>
+  </si>
+  <si>
+    <t>Needs Help</t>
+  </si>
+  <si>
+    <t>some_asst</t>
+  </si>
+  <si>
+    <t>Some Asst</t>
+  </si>
+  <si>
+    <t>full_asst</t>
+  </si>
+  <si>
+    <t>Full Asst</t>
+  </si>
+  <si>
+    <t>practical_inadequate</t>
+  </si>
+  <si>
+    <t>practical_some_asst</t>
+  </si>
+  <si>
+    <t>practical_limitted</t>
+  </si>
+  <si>
+    <t>practical_unable</t>
+  </si>
+  <si>
+    <t>activities_regular</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>activities_needs</t>
+  </si>
+  <si>
+    <t>Needs</t>
+  </si>
+  <si>
+    <t>activities_resists</t>
+  </si>
+  <si>
+    <t>Resists</t>
+  </si>
+  <si>
+    <t>activities_isolated</t>
+  </si>
+  <si>
+    <t>Isolated</t>
+  </si>
+  <si>
+    <t>dental_none</t>
+  </si>
+  <si>
+    <t>dental_minor</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>dental_moderate</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>dental_major</t>
+  </si>
+  <si>
+    <t>Major</t>
   </si>
   <si>
     <t>form_title</t>
@@ -640,10 +783,10 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -885,7 +1028,7 @@
     <col customWidth="1" min="1" max="1" width="28.63"/>
     <col customWidth="1" min="2" max="2" width="19.63"/>
     <col customWidth="1" min="3" max="4" width="31.63"/>
-    <col customWidth="1" min="5" max="5" width="141.63"/>
+    <col customWidth="1" min="5" max="5" width="157.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1702,65 +1845,130 @@
       <c r="D30" s="4"/>
       <c r="E30" s="16"/>
     </row>
-    <row r="31" ht="145.5" customHeight="1">
+    <row r="31" ht="18.75" customHeight="1">
       <c r="A31" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" ht="18.75" customHeight="1">
+      <c r="A32" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" ht="18.75" customHeight="1">
+      <c r="A33" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" ht="18.75" customHeight="1">
+      <c r="A34" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" ht="18.75" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" ht="224.25" customHeight="1">
+      <c r="A36" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="18" t="s">
+      <c r="B36" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="16"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
+      <c r="B37" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="17"/>
+      <c r="E38" s="16"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="17"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="4"/>
+    <row r="41">
+      <c r="A41" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1778,11 +1986,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
+    <col customWidth="1" min="2" max="2" width="20.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
@@ -1796,10 +2005,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">
@@ -1807,10 +2016,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -1818,10 +2027,10 @@
         <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
@@ -1829,10 +2038,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
@@ -1840,10 +2049,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
@@ -1851,10 +2060,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -1862,10 +2071,10 @@
         <v>41</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
@@ -1873,10 +2082,10 @@
         <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
@@ -1884,10 +2093,10 @@
         <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
@@ -1895,10 +2104,10 @@
         <v>44</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -1906,10 +2115,10 @@
         <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -1917,54 +2126,54 @@
         <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
@@ -1972,10 +2181,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19">
@@ -1983,10 +2192,10 @@
         <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20">
@@ -1994,10 +2203,10 @@
         <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
@@ -2005,10 +2214,10 @@
         <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
@@ -2016,10 +2225,10 @@
         <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23">
@@ -2027,10 +2236,10 @@
         <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24">
@@ -2038,10 +2247,10 @@
         <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -2049,10 +2258,10 @@
         <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -2060,10 +2269,10 @@
         <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27">
@@ -2071,10 +2280,10 @@
         <v>56</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28">
@@ -2082,10 +2291,10 @@
         <v>56</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29">
@@ -2093,10 +2302,10 @@
         <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30">
@@ -2104,10 +2313,10 @@
         <v>59</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31">
@@ -2115,10 +2324,10 @@
         <v>59</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32">
@@ -2126,10 +2335,10 @@
         <v>59</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33">
@@ -2137,10 +2346,10 @@
         <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34">
@@ -2148,10 +2357,10 @@
         <v>62</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35">
@@ -2159,10 +2368,10 @@
         <v>62</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36">
@@ -2170,10 +2379,230 @@
         <v>62</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>140</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2198,28 +2627,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="G1" s="22"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>35</v>
@@ -2228,13 +2657,13 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:redesigning the level of care assessment form by adding in more fields
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="235">
   <si>
     <t>type</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Transportation</t>
+  </si>
+  <si>
+    <t>select_one party</t>
+  </si>
+  <si>
+    <t>party</t>
+  </si>
+  <si>
+    <t>3rd Party Assistance</t>
   </si>
   <si>
     <t>select_one support</t>
@@ -275,6 +284,13 @@
   </si>
   <si>
     <t xml:space="preserve"> if((${score} &gt;= 1 and ${score} &lt;= 15), 'Limitted', if((${score} &gt;= 16  and ${score} &lt; 40 ), 'Supportive', if((${score} &gt;= 40), 'Comprehensive','')))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant Findings 
+</t>
   </si>
   <si>
     <t>note</t>
@@ -306,79 +322,118 @@
     <t>Risk Category is:${category}</t>
   </si>
   <si>
+    <t>note_1</t>
+  </si>
+  <si>
+    <t>15 = Limited 	 	 Cases reviewed as needed, but at least annually</t>
+  </si>
+  <si>
+    <t>note_2</t>
+  </si>
+  <si>
+    <t>16-40 = Supportive 	 Cases reviewed at least every 6 months</t>
+  </si>
+  <si>
+    <t>note_3</t>
+  </si>
+  <si>
+    <t>40+ Comprehensive 	 Cases reviewed at least twice every month</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_assesment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Date of Level of Care Assessment:</t>
+  </si>
+  <si>
+    <t>today()</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
     <t>zero</t>
   </si>
   <si>
-    <t>CD4&gt;500</t>
+    <t xml:space="preserve">In Care - CD4 &gt;500; viral load &lt;100/undetectable; in care, medically stable, and adheres to appointments without CM oversight; chronic condition under control with medication and/or treatment
+</t>
   </si>
   <si>
     <t>two</t>
   </si>
   <si>
-    <t>CD4 200-499</t>
+    <t xml:space="preserve">Occasional - CD4 200-499; viral load 100-9,999; lab values stable; in care, generally medically stable, and adheres to appointments with CM assistance &lt;30% of time; may have minor conditions requiring treatment
+</t>
   </si>
   <si>
     <t>five</t>
   </si>
   <si>
-    <t>CD4 50-199</t>
+    <t>Frequent - CD4 50-199; viral load 10,000-100,000; lab values stable/ improving; no new side effects/ current side effects being controlled; inconsistent appointments, medically unstable, and CM intervention needed 30-74% of time</t>
   </si>
   <si>
     <t>fifty</t>
   </si>
   <si>
-    <t>CD4&lt;50</t>
+    <t xml:space="preserve">Poor in care - CD4 &lt;50; viral load &gt;100,000; lab values deteriorating; physical side effects increasing; new health issues emerging; medically unstable or unknown (newly diagnosed); not in care or CM intervention need &gt;75% of appointments; pregnant female
+</t>
   </si>
   <si>
     <t>good</t>
   </si>
   <si>
-    <t>Good</t>
+    <t xml:space="preserve">Good - Effectively demonstrates knowledge of HIV disease and treatment </t>
   </si>
   <si>
     <t>some_what</t>
   </si>
   <si>
-    <t>Somewhat</t>
+    <t xml:space="preserve">Somewhat - Can discuss knowledge and understanding of HIV; may have some misconceptions but listens when addressed
+</t>
   </si>
   <si>
     <t>little</t>
   </si>
   <si>
-    <t>Little</t>
+    <t xml:space="preserve">Little - Cannot fully communicate concerning HIV may have cultural or other barriers
+</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>None</t>
+    <t xml:space="preserve">None - Cannot or will not communicate concerning HIV; barriers cannot be fully addressed
+</t>
   </si>
   <si>
     <t>always</t>
   </si>
   <si>
-    <t>Always</t>
+    <t xml:space="preserve">Always - Always adheres to treatment; clearly communicates importance; no side effects or side effects are not interrupting activities of daily living; obtains meds without assistance; willingly participates in care plan
+</t>
   </si>
   <si>
     <t>usually</t>
   </si>
   <si>
-    <t>Usually</t>
+    <t>Usually - usually adheres to treatment; fair communication of importance; side effects are minimally impacting daily activities; participates in care plan</t>
   </si>
   <si>
     <t>rarely</t>
   </si>
   <si>
-    <t>Rarely</t>
+    <t xml:space="preserve">Rarely - Sometimes adheres to treatment; reflects little understanding or willingness to comply; side effects moderately impacting daily activities; does not readily participate in plan but follows most directives
+</t>
   </si>
   <si>
     <t>never</t>
   </si>
   <si>
-    <t>Never</t>
+    <t xml:space="preserve">Never - Rarely adheres to treatment; cannot communicate understanding of compliance; numerous side effects severely impacting daily activities; cannot or will not participate in plan; compliance issues
+</t>
   </si>
   <si>
     <t xml:space="preserve">mental </t>
@@ -387,220 +442,332 @@
     <t>no_history</t>
   </si>
   <si>
-    <t>No history</t>
+    <t xml:space="preserve">No history - No history of mental illness or violence/abuse; no family history
+</t>
   </si>
   <si>
     <t>has_access</t>
   </si>
   <si>
-    <t>Has access</t>
+    <t xml:space="preserve">Has access - History of illness or abuse but connected and compliant with treatment; may need some support or counseling but otherwise functional 
+</t>
   </si>
   <si>
     <t>failed_treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">Failed treatment </t>
+    <t xml:space="preserve">Failed treatment - History of illness or abuse; needs high level of emotional support; connected with treatment but may have compliance issues; experiencing stress 
+</t>
   </si>
   <si>
     <t xml:space="preserve">serious </t>
   </si>
   <si>
-    <t>Serious</t>
+    <t xml:space="preserve">Serious - History of illness or abuse; active problems and crisis; requires significant emotional support and therapy but not accessing it; high stress; not functional
+</t>
   </si>
   <si>
     <t>consistent</t>
   </si>
   <si>
-    <t>Consistent</t>
+    <t xml:space="preserve">Consistent - Has own/other means of transportation consistently available 
+</t>
   </si>
   <si>
     <t>questionable</t>
   </si>
   <si>
-    <t>Questionable</t>
+    <t xml:space="preserve">Questionable - Has general access to public/private transportation; must occasionally rely on others 
+</t>
   </si>
   <si>
     <t>irregular</t>
   </si>
   <si>
-    <t>Irregular</t>
+    <t xml:space="preserve">Irregular - Has irregular access to public/private transportation 
+</t>
   </si>
   <si>
     <t>transportation_none</t>
   </si>
   <si>
+    <t xml:space="preserve">None - Public/private transportation unavailable
+</t>
+  </si>
+  <si>
+    <t>enrolled</t>
+  </si>
+  <si>
+    <t>Enrolled - Has independently completed all necessary paperwork and received approval; no longer has need beyond possible annual reapplication</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Pending -Completed necessary forms with limited assistance from CM; forms submitted; approval pending</t>
+  </si>
+  <si>
+    <t>will_apply</t>
+  </si>
+  <si>
+    <t>Will Apply - Needs assistance from CM to complete forms; requires regular reminders; forms yet to be submitted or denied for reasons other than need</t>
+  </si>
+  <si>
+    <t>denied</t>
+  </si>
+  <si>
+    <t>Denied -Needs assistance from CM to complete forms; will not meet with CM to complete; forms late for submission; application denied</t>
+  </si>
+  <si>
     <t>reliable</t>
   </si>
   <si>
-    <t>Reliable</t>
+    <t xml:space="preserve">Reliable - Has reliable friends/family to provide ongoing support
+</t>
   </si>
   <si>
     <t>only</t>
   </si>
   <si>
-    <t>Crisis only</t>
+    <t xml:space="preserve">Questionable - Often has help, but not always reliable; in jeopardy if/when HIV status is divulged
+</t>
+  </si>
+  <si>
+    <t>crisis_only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crisis only - Some support in a crisis only; resists group involvement 
+</t>
+  </si>
+  <si>
+    <t>suppport</t>
   </si>
   <si>
     <t>support_none</t>
   </si>
   <si>
+    <t>None -No reliable support when needed; support group unavailable</t>
+  </si>
+  <si>
     <t>communication_good</t>
   </si>
   <si>
+    <t xml:space="preserve">Good - Can effectively communicate concerns with CM; no language, sensory, cultural, or other barriers to care 
+</t>
+  </si>
+  <si>
     <t>temporary</t>
   </si>
   <si>
-    <t>Temporary</t>
+    <t xml:space="preserve">Fair- Can generally communicate with CM; can read written materials and communicate understanding; no other barriers 
+</t>
   </si>
   <si>
     <t>limitted</t>
   </si>
   <si>
-    <t>Limitted</t>
+    <t xml:space="preserve">Limited - Difficulty communicating with CM; cannot read written materials as provided; English not first language; interpreter needed at all appointments 
+</t>
   </si>
   <si>
     <t>communication_none</t>
   </si>
   <si>
+    <t xml:space="preserve">None - Extreme difficulty communicating with CM; interpreter necessary but unavailable; barrier to care but cannot be easily resolved
+</t>
+  </si>
+  <si>
     <t>employed</t>
   </si>
   <si>
-    <t>Employed</t>
+    <t xml:space="preserve">Employed - Stably employed, regularly meets expenses 
+</t>
   </si>
   <si>
     <t>ltd_probs</t>
   </si>
   <si>
-    <t>Ltd Probs</t>
+    <t xml:space="preserve">Temporary - Under- or temporarily employed; able and wants to work; has some job seeking skills 
+</t>
   </si>
   <si>
     <t>unemployed</t>
   </si>
   <si>
-    <t>Unemployed</t>
+    <t xml:space="preserve">Unemployed -Unemployed or job threatened by HIV disease; able and wants to work at suitable job 
+</t>
   </si>
   <si>
     <t>unable</t>
   </si>
   <si>
-    <t>Unable</t>
+    <t xml:space="preserve">Unable - Unemployed or unable to work on regular basis; no job-seeking skills
+</t>
   </si>
   <si>
     <t>self_managed</t>
   </si>
   <si>
-    <t>Self-managed</t>
+    <t xml:space="preserve">Self-managed -Has safe, stable, and clean living situation and has self-managed options 
+</t>
   </si>
   <si>
     <t>adequate</t>
   </si>
   <si>
-    <t>Adequate</t>
+    <t xml:space="preserve">Adequate (Ltd Probs) -Has safe, stable, and clean living arrangement; externally controlled; payment up-to-date; limited self-managed options; known stressors may necessitate relocation 
+</t>
   </si>
   <si>
     <t>unsafe</t>
   </si>
   <si>
-    <t>Unsafe</t>
+    <t xml:space="preserve">Unsafe -Housing unsafe, unstable, or ill-kept; week-to-week occupancy; no personal control; payments behind, or in temporary shelter; no self-managed options 
+</t>
   </si>
   <si>
     <t>homless</t>
   </si>
   <si>
-    <t>Homeless</t>
+    <t xml:space="preserve">Homeless -Facing imminent eviction or no place to live currently; NO self-managed options
+</t>
   </si>
   <si>
     <t>financial_stable</t>
   </si>
   <si>
-    <t>Stable</t>
+    <t xml:space="preserve">Stable -Stable income/benefits adequate to meet needs; completes all necessary/ applicable benefit documents
+</t>
   </si>
   <si>
     <t>financial_adequate</t>
   </si>
   <si>
+    <t xml:space="preserve">Adequate -Adequate income; needs some help completing benefit documents; medical state may jeopardize income 
+</t>
+  </si>
+  <si>
     <t>financial_inadequate</t>
   </si>
   <si>
-    <t>Inadequate</t>
+    <t xml:space="preserve">Inadequate -Inadequate current resources; has not applied for benefits or awaiting benefit determination 
+</t>
   </si>
   <si>
     <t>financial_none</t>
   </si>
   <si>
+    <t xml:space="preserve">None- No current resources; requires help to understand/complete benefit documents or benefits denied
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None - All necessary legal documents completed
+</t>
+  </si>
+  <si>
     <t>needs_help</t>
   </si>
   <si>
-    <t>Needs Help</t>
+    <t xml:space="preserve">Needs Help - Needs some help completing standard documents
+</t>
   </si>
   <si>
     <t>some_asst</t>
   </si>
   <si>
-    <t>Some Asst</t>
+    <t xml:space="preserve">Some Assistance -Requires assistance with many documents 
+</t>
   </si>
   <si>
     <t>full_asst</t>
   </si>
   <si>
-    <t>Full Asst</t>
+    <t xml:space="preserve">Full Assistance - Requires help understanding and completing most documents
+</t>
   </si>
   <si>
     <t>practical_inadequate</t>
   </si>
   <si>
+    <t xml:space="preserve">Independent -Able to independently provide for own needs and perform all activities of daily living (ADLs) 
+</t>
+  </si>
+  <si>
     <t>practical_some_asst</t>
   </si>
   <si>
+    <t xml:space="preserve">Some Assistance  -Can provide for some ADLs and arrange for the rest; may have dependent children not living in household
+</t>
+  </si>
+  <si>
     <t>practical_limitted</t>
   </si>
   <si>
+    <t xml:space="preserve">Limited -Limited capacity for arranging ADLs on a regular basis; dependent children in household with another adult in parental role 
+</t>
+  </si>
+  <si>
     <t>practical_unable</t>
   </si>
   <si>
+    <t xml:space="preserve">Unable - Unable to arrange for food, clothing, and other ADLs; client is a dependent child or has sole responsibility for dependent(s) in household
+</t>
+  </si>
+  <si>
     <t>activities_regular</t>
   </si>
   <si>
-    <t>Regular</t>
+    <t xml:space="preserve">Regular -Regular involvement in spiritual, leisure, or other SSAs
+</t>
   </si>
   <si>
     <t>activities_needs</t>
   </si>
   <si>
-    <t>Needs</t>
+    <t xml:space="preserve">Needs -Needs education/exposure to SSAs 
+</t>
   </si>
   <si>
     <t>activities_resists</t>
   </si>
   <si>
-    <t>Resists</t>
+    <t xml:space="preserve">Resists -Actively resists SSAs involvement
+</t>
   </si>
   <si>
     <t>activities_isolated</t>
   </si>
   <si>
-    <t>Isolated</t>
+    <t xml:space="preserve">Isolated -Isolated from suitable SSAs
+</t>
   </si>
   <si>
     <t>dental_none</t>
   </si>
   <si>
+    <t xml:space="preserve">None - No dental needs beyond regular check-ups; has pay source
+</t>
+  </si>
+  <si>
     <t>dental_minor</t>
   </si>
   <si>
-    <t>Minor</t>
+    <t xml:space="preserve">Minor -Minor dental needs; may need assistance from 3rd party payor 
+</t>
   </si>
   <si>
     <t>dental_moderate</t>
   </si>
   <si>
-    <t>Moderate</t>
+    <t xml:space="preserve">Moderate Significant dental needs affecting other health; needs pay source 
+</t>
   </si>
   <si>
     <t>dental_major</t>
   </si>
   <si>
-    <t>Major</t>
+    <t xml:space="preserve">Major - Major dental needs; needs pay source or denied; noncompliant in correcting issues 
+</t>
   </si>
   <si>
     <t>form_title</t>
@@ -637,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -677,6 +844,12 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -730,7 +903,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -750,20 +923,29 @@
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -995,7 +1177,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="28.63"/>
     <col customWidth="1" min="2" max="2" width="19.63"/>
-    <col customWidth="1" min="3" max="4" width="31.63"/>
+    <col customWidth="1" min="3" max="3" width="44.38"/>
+    <col customWidth="1" min="4" max="4" width="31.63"/>
     <col customWidth="1" min="5" max="5" width="167.88"/>
     <col customWidth="1" min="6" max="6" width="12.63"/>
   </cols>
@@ -1763,13 +1946,13 @@
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="3"/>
@@ -1814,137 +1997,211 @@
       <c r="D30" s="3"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" ht="18.75" customHeight="1">
-      <c r="A31" s="9" t="s">
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="9"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="9"/>
+      <c r="D32" s="10"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="9"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="18.75" customHeight="1">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="9"/>
+      <c r="D34" s="10"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="18.75" customHeight="1">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="9"/>
+      <c r="D35" s="10"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" ht="224.25" customHeight="1">
-      <c r="A36" s="9" t="s">
+    <row r="36" ht="18.75" customHeight="1">
+      <c r="A36" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" ht="224.25" customHeight="1">
+      <c r="A37" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9" t="s">
+      <c r="B37" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="9"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="3"/>
+    </row>
     <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
@@ -2898,6 +3155,12 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2915,17 +3178,18 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.75"/>
     <col customWidth="1" min="2" max="2" width="20.13"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
+    <col customWidth="1" min="3" max="3" width="155.88"/>
+    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2934,10 +3198,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>90</v>
+        <v>104</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -2945,10 +3209,10 @@
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>106</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -2956,10 +3220,10 @@
         <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>108</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -2967,10 +3231,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>96</v>
+        <v>110</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -2978,10 +3242,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>112</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -2989,10 +3253,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>100</v>
+        <v>114</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -3000,10 +3264,10 @@
         <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>102</v>
+        <v>116</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -3011,10 +3275,10 @@
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>104</v>
+        <v>118</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -3022,10 +3286,10 @@
         <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>106</v>
+        <v>120</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -3033,10 +3297,10 @@
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>122</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -3044,10 +3308,10 @@
         <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>110</v>
+        <v>124</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -3055,54 +3319,54 @@
         <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>112</v>
+        <v>126</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>117</v>
+        <v>131</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>121</v>
+        <v>135</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -3110,10 +3374,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>123</v>
+        <v>137</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -3121,10 +3385,10 @@
         <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>125</v>
+        <v>139</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -3132,76 +3396,76 @@
         <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>104</v>
+      <c r="B21" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>130</v>
+      <c r="B22" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>132</v>
+      <c r="B23" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>104</v>
+      <c r="B24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B26" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>136</v>
+        <v>153</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -3209,98 +3473,98 @@
         <v>56</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>138</v>
+        <v>155</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>104</v>
+      <c r="B28" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>141</v>
+      <c r="A29" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>143</v>
+      <c r="B30" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>145</v>
+        <v>164</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>147</v>
+        <v>166</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="4" t="s">
+      <c r="B34" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="B35" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>153</v>
+        <v>172</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -3308,21 +3572,21 @@
         <v>62</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>155</v>
+        <v>174</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>157</v>
+        <v>176</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -3330,43 +3594,43 @@
         <v>65</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>151</v>
+        <v>178</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>160</v>
+        <v>180</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>104</v>
+        <v>182</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>104</v>
+        <v>184</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -3374,10 +3638,10 @@
         <v>68</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>163</v>
+        <v>186</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -3385,10 +3649,10 @@
         <v>68</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>165</v>
+        <v>188</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -3396,21 +3660,21 @@
         <v>68</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>167</v>
+        <v>190</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>160</v>
+        <v>192</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -3418,10 +3682,10 @@
         <v>71</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>165</v>
+        <v>118</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -3429,10 +3693,10 @@
         <v>71</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>138</v>
+        <v>195</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -3440,21 +3704,21 @@
         <v>71</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>147</v>
+        <v>197</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>173</v>
+        <v>199</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -3462,10 +3726,10 @@
         <v>74</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -3473,10 +3737,10 @@
         <v>74</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>177</v>
+        <v>203</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -3484,21 +3748,21 @@
         <v>74</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>179</v>
+        <v>205</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>104</v>
+        <v>207</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -3506,10 +3770,10 @@
         <v>77</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>182</v>
+        <v>209</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -3517,10 +3781,10 @@
         <v>77</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>184</v>
+        <v>211</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -3528,17 +3792,67 @@
         <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
+        <v>213</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
@@ -4478,6 +4792,11 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4501,28 +4820,28 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" s="14"/>
+        <v>229</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>35</v>
@@ -4531,13 +4850,13 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
auto:adding the ability to automatically switch to a comprehensive risk category when certain fields are selected
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -264,10 +264,10 @@
     <t>score</t>
   </si>
   <si>
-    <t xml:space="preserve">if(selected(${medical}, 'zero'), 1, 0) + if(selected(${medical}, 'two'), 2, 0) + if(selected(${medical}, 'five'), 3, 0) + if(selected(${medical}, 'fifty'), 4, 0) + 
- if(selected(${knowledge}, 'good'), 1, 0) + if(selected(${knowledge}, 'some_what'), 2, 0) + if(selected(${knowledge}, 'little'), 3, 0) + if(selected(${knowledge}, 'none'), 4, 0) + 
+    <t xml:space="preserve">if(selected(${medical}, 'zero'), 1, 0) + if(selected(${medical}, 'two'), 2, 0) + if(selected(${medical}, 'five'), 40, 0) + if(selected(${medical}, 'fifty'), 40, 0) + 
+ if(selected(${knowledge}, 'good'), 1, 0) + if(selected(${knowledge}, 'some_what'), 2, 0) + if(selected(${knowledge}, 'little'), 40, 0) + if(selected(${knowledge}, 'none'), 40, 0) + 
  if(selected(${adherence}, 'always'), 1, 0) + if(selected(${adherence}, 'usually'), 2, 0) + if(selected(${adherence}, 'rarely'), 3, 0) + if(selected(${adherence}, 'never'), 4, 0) + 
- if(selected(${mental}, 'no_history'), 1, 0) + if(selected(${mental}, 'has_access'), 2, 0) + if(selected(${mental}, 'failed_treatment'), 3, 0) + if(selected(${mental}, 'serious'), 4, 0) + 
+ if(selected(${mental}, 'no_history'), 1, 0) + if(selected(${mental}, 'has_access'), 2, 0) + if(selected(${mental}, 'failed_treatment'), 40, 0) + if(selected(${mental}, 'serious'), 40, 0) + 
  if(selected(${transportation}, 'consistent'), 1, 0) + if(selected(${transportation}, 'questionable'), 2, 0) + if(selected(${transportation}, 'irregular'), 3, 0) + if(selected(${transportation}, 'transportation_none'), 4, 0) + 
   if(selected(${financial}, 'financial_stable'), 1, 0) + if(selected(${financial}, 'financial_adequate'), 2, 0) + if(selected(${financial}, 'financial_inadequate'), 3, 0) + if(selected(${financial}, 'financial_none'), 4, 0) + 
  if(selected(${legal}, 'none'), 1, 0) + if(selected(${legal}, 'needs_help'), 2, 0) + if(selected(${legal}, 'some_asst'), 3, 0) + if(selected(${legal}, 'full_asst'), 4, 0) + 

</xml_diff>

<commit_message>
auto:changing the level of care assessment form to reflect data from the enrollment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="270">
   <si>
     <t>type</t>
   </si>
@@ -93,6 +93,18 @@
     <t>sex</t>
   </si>
   <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -120,10 +132,107 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>patient_name1</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name1</t>
+  </si>
+  <si>
+    <t>patient_aka</t>
+  </si>
+  <si>
+    <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_at</t>
+  </si>
+  <si>
+    <t>../inputs/contact/at</t>
+  </si>
+  <si>
+    <t>patient_date_of_birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth </t>
+  </si>
+  <si>
+    <t>../inputs/contact/date_of_birth</t>
+  </si>
+  <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)</t>
+  </si>
+  <si>
+    <t>last_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/lstname != '', instance('contact-summary')/context/lstname, .)</t>
+  </si>
+  <si>
+    <t>date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
+  </si>
+  <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
+    <t>at_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_at != '', instance('contact-summary')/context/patient_at, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
     <t>care</t>
   </si>
   <si>
     <t>Questionaire</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>${tsis_ctx}</t>
   </si>
   <si>
     <t>select_one medical</t>
@@ -291,9 +400,6 @@
   <si>
     <t xml:space="preserve">Significant Findings 
 </t>
-  </si>
-  <si>
-    <t>note</t>
   </si>
   <si>
     <t>score_note</t>
@@ -903,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -920,6 +1026,12 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1533,18 +1645,19 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1567,18 +1680,19 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1601,17 +1715,16 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
       <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1637,17 +1750,16 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
       <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1674,10 +1786,14 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
@@ -1704,10 +1820,14 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
@@ -1733,14 +1853,20 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1763,14 +1889,20 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1793,20 +1925,19 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>30</v>
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1829,20 +1960,19 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>33</v>
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1865,366 +1995,1115 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3" t="s">
+      <c r="B41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="3" t="s">
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" s="10" t="s">
+      <c r="B42" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="9"/>
+      <c r="Z42" s="9"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" s="10" t="s">
+      <c r="C43" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C44" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" ht="18.75" customHeight="1">
-      <c r="A34" s="10" t="s">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="9"/>
+      <c r="Z44" s="9"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B45" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C45" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" ht="18.75" customHeight="1">
-      <c r="A35" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" ht="18.75" customHeight="1">
-      <c r="A36" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" ht="224.25" customHeight="1">
-      <c r="A37" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11" t="s">
-        <v>102</v>
-      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
+      <c r="A47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" ht="18.75" customHeight="1">
+      <c r="A55" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" ht="18.75" customHeight="1">
+      <c r="A56" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" ht="18.75" customHeight="1">
+      <c r="A57" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" ht="18.75" customHeight="1">
+      <c r="A58" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" ht="18.75" customHeight="1">
+      <c r="A59" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" ht="224.25" customHeight="1">
+      <c r="A60" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" ht="15.75" customHeight="1">
+      <c r="A65" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="12"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="12"/>
+      <c r="E68" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="3"/>
+    </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1"/>
@@ -3161,6 +4040,29 @@
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
+    <row r="1020" ht="15.75" customHeight="1"/>
+    <row r="1021" ht="15.75" customHeight="1"/>
+    <row r="1022" ht="15.75" customHeight="1"/>
+    <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3183,674 +4085,674 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>105</v>
+        <v>139</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>109</v>
+        <v>143</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>111</v>
+        <v>145</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>113</v>
+        <v>147</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>115</v>
+        <v>149</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>117</v>
+        <v>151</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>119</v>
+        <v>153</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>121</v>
+        <v>155</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>123</v>
+        <v>157</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>125</v>
+        <v>159</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>127</v>
+        <v>161</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>130</v>
+        <v>164</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>132</v>
+        <v>166</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>134</v>
+        <v>168</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>136</v>
+        <v>170</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>138</v>
+        <v>172</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>140</v>
+        <v>174</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>142</v>
+        <v>176</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>144</v>
+        <v>86</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>146</v>
+      <c r="A22" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>148</v>
+      <c r="A23" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>150</v>
+      <c r="A24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>152</v>
+      <c r="A25" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>154</v>
+        <v>188</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>156</v>
+        <v>190</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>158</v>
+        <v>92</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>161</v>
+      <c r="A29" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>163</v>
+        <v>95</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>165</v>
+        <v>199</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>167</v>
+        <v>201</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>169</v>
+        <v>95</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>171</v>
+        <v>205</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>173</v>
+        <v>207</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>175</v>
+        <v>209</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>177</v>
+        <v>211</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>179</v>
+        <v>213</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>181</v>
+        <v>215</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>183</v>
+        <v>217</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>185</v>
+        <v>219</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>187</v>
+        <v>221</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>189</v>
+        <v>223</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>191</v>
+        <v>225</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>193</v>
+        <v>227</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>194</v>
+        <v>153</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>196</v>
+        <v>230</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>198</v>
+        <v>232</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>200</v>
+        <v>234</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>202</v>
+        <v>236</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>204</v>
+        <v>238</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>206</v>
+        <v>240</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>208</v>
+        <v>242</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>210</v>
+        <v>244</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>212</v>
+        <v>246</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>214</v>
+        <v>248</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>216</v>
+        <v>250</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>218</v>
+        <v>252</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>220</v>
+        <v>254</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>222</v>
+        <v>256</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>224</v>
+        <v>258</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
@@ -4820,43 +5722,43 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="G1" s="17"/>
+        <v>264</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>231</v>
+        <v>266</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
auto:add patient identifier card in the level of care assessment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="278">
   <si>
     <t>type</t>
   </si>
@@ -105,6 +105,9 @@
     <t>at</t>
   </si>
   <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -154,6 +157,12 @@
   </si>
   <si>
     <t>../inputs/contact/at</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
   </si>
   <si>
     <t>patient_date_of_birth</t>
@@ -208,12 +217,15 @@
 </t>
   </si>
   <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>care</t>
   </si>
   <si>
-    <t>Questionaire</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -223,16 +235,28 @@
     <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
   </si>
   <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>${aka_ctx}  |  ${yr_date_of_birth_ctx} yr   ${at_ctx}</t>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
   </si>
   <si>
     <t>dob</t>
   </si>
   <si>
-    <t>${tsis_ctx}</t>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>select_one medical</t>
@@ -1009,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1027,16 +1051,22 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -1289,9 +1319,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="28.63"/>
     <col customWidth="1" min="2" max="2" width="19.63"/>
-    <col customWidth="1" min="3" max="3" width="44.38"/>
-    <col customWidth="1" min="4" max="4" width="31.63"/>
-    <col customWidth="1" min="5" max="5" width="167.88"/>
+    <col customWidth="1" min="3" max="3" width="27.38"/>
+    <col customWidth="1" min="4" max="4" width="30.88"/>
+    <col customWidth="1" min="5" max="5" width="163.88"/>
     <col customWidth="1" min="6" max="6" width="12.63"/>
   </cols>
   <sheetData>
@@ -1785,18 +1815,20 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1823,7 +1855,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>14</v>
@@ -1853,20 +1885,18 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
+      <c r="A17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1893,7 +1923,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>14</v>
@@ -1925,16 +1955,17 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1964,7 +1995,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1999,7 +2030,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
@@ -2034,7 +2065,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
@@ -2065,14 +2096,19 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -2096,7 +2132,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
@@ -2126,7 +2162,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -2156,7 +2192,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
@@ -2188,16 +2224,10 @@
       <c r="A27" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -2222,17 +2252,17 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2257,23 +2287,25 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2292,17 +2324,17 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2326,17 +2358,17 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2360,17 +2392,17 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2394,17 +2426,17 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2428,22 +2460,24 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>51</v>
+      <c r="E34" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2462,17 +2496,17 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2496,17 +2530,17 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="8" t="s">
-        <v>55</v>
+      <c r="E36" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -2530,17 +2564,17 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2564,17 +2598,17 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
-        <v>59</v>
+      <c r="E38" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2598,17 +2632,17 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2632,17 +2666,17 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2665,450 +2699,617 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="9"/>
-      <c r="U42" s="9"/>
-      <c r="V42" s="9"/>
-      <c r="W42" s="9"/>
-      <c r="X42" s="9"/>
-      <c r="Y42" s="9"/>
-      <c r="Z42" s="9"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
-      <c r="X43" s="9"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="9"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="3" t="s">
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+      <c r="Z45" s="8"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="8"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8"/>
+      <c r="Z47" s="8"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="3" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="8"/>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+      <c r="V49" s="8"/>
+      <c r="W49" s="8"/>
+      <c r="X49" s="8"/>
+      <c r="Y49" s="8"/>
+      <c r="Z49" s="8"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="D50" s="3"/>
-      <c r="E50" s="10"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="10"/>
+        <v>85</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D52" s="3"/>
-      <c r="E52" s="10"/>
+      <c r="E52" s="13"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D53" s="3"/>
-      <c r="E53" s="10"/>
+      <c r="E53" s="13"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="13"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D56" s="3"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" ht="18.75" customHeight="1">
-      <c r="A55" s="12" t="s">
+      <c r="B57" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="C57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="D57" s="3"/>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" ht="18.75" customHeight="1">
-      <c r="A56" s="12" t="s">
+      <c r="B58" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="C58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="D58" s="3"/>
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="10"/>
-    </row>
-    <row r="57" ht="18.75" customHeight="1">
-      <c r="A57" s="12" t="s">
+      <c r="B59" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="C59" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="D59" s="3"/>
+      <c r="E59" s="13"/>
+    </row>
+    <row r="60" ht="18.75" customHeight="1">
+      <c r="A60" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" ht="18.75" customHeight="1">
-      <c r="A58" s="12" t="s">
+      <c r="B60" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="C60" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="D60" s="14"/>
+      <c r="E60" s="13"/>
+    </row>
+    <row r="61" ht="18.75" customHeight="1">
+      <c r="A61" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" ht="18.75" customHeight="1">
-      <c r="A59" s="12" t="s">
+      <c r="B61" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="C61" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="D61" s="14"/>
+      <c r="E61" s="13"/>
+    </row>
+    <row r="62" ht="18.75" customHeight="1">
+      <c r="A62" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" ht="224.25" customHeight="1">
-      <c r="A60" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="12" t="s">
+      <c r="B62" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="13" t="s">
+      <c r="C62" s="14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="12" t="s">
+      <c r="D62" s="14"/>
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" ht="18.75" customHeight="1">
+      <c r="A63" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="10" t="s">
+      <c r="B63" s="14" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="D63" s="14"/>
+      <c r="E63" s="13"/>
+    </row>
+    <row r="64" ht="18.75" customHeight="1">
+      <c r="A64" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="10"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="12" t="s">
+      <c r="B64" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C64" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="12" t="s">
+      <c r="D64" s="14"/>
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" ht="224.25" customHeight="1">
+      <c r="A65" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B66" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C67" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="12"/>
-      <c r="E67" s="10"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="13"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="14"/>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="C69" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="D69" s="14"/>
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="13" t="s">
+      <c r="C70" s="16" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="13"/>
+    </row>
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="13"/>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="14"/>
+      <c r="E73" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="3"/>
+    </row>
     <row r="76" ht="15.75" customHeight="1"/>
     <row r="77" ht="15.75" customHeight="1"/>
     <row r="78" ht="15.75" customHeight="1"/>
@@ -4063,6 +4264,11 @@
     <row r="1027" ht="15.75" customHeight="1"/>
     <row r="1028" ht="15.75" customHeight="1"/>
     <row r="1029" ht="15.75" customHeight="1"/>
+    <row r="1030" ht="15.75" customHeight="1"/>
+    <row r="1031" ht="15.75" customHeight="1"/>
+    <row r="1032" ht="15.75" customHeight="1"/>
+    <row r="1033" ht="15.75" customHeight="1"/>
+    <row r="1034" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4085,674 +4291,674 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>140</v>
+        <v>147</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>142</v>
+        <v>149</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>144</v>
+        <v>151</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>146</v>
+        <v>153</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>148</v>
+        <v>155</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>152</v>
+        <v>159</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>154</v>
+        <v>161</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>156</v>
+        <v>163</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>158</v>
+        <v>165</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>160</v>
+        <v>167</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>162</v>
+        <v>169</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>165</v>
+        <v>172</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>167</v>
+        <v>174</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>169</v>
+        <v>176</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>173</v>
+        <v>180</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>175</v>
+        <v>182</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>177</v>
+        <v>184</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>179</v>
+        <v>94</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>181</v>
+      <c r="A22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>183</v>
+      <c r="A23" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>185</v>
+      <c r="A24" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>187</v>
+      <c r="A25" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>189</v>
+        <v>196</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>191</v>
+        <v>198</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>193</v>
+        <v>100</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>196</v>
+      <c r="A29" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>198</v>
+        <v>103</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>200</v>
+        <v>207</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>202</v>
+        <v>209</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>204</v>
+        <v>103</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>206</v>
+        <v>213</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>208</v>
+        <v>215</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>210</v>
+        <v>217</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>212</v>
+        <v>219</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>214</v>
+        <v>221</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>216</v>
+        <v>223</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>218</v>
+        <v>225</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>220</v>
+        <v>227</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>222</v>
+        <v>229</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>226</v>
+        <v>233</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>228</v>
+        <v>235</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>229</v>
+        <v>161</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>231</v>
+        <v>238</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>233</v>
+        <v>240</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>235</v>
+        <v>242</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>237</v>
+        <v>244</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>239</v>
+        <v>246</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>241</v>
+        <v>248</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>243</v>
+        <v>250</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>245</v>
+        <v>252</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>247</v>
+        <v>254</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>249</v>
+        <v>256</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>251</v>
+        <v>258</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>253</v>
+        <v>260</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>255</v>
+        <v>262</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>257</v>
+        <v>264</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>259</v>
+        <v>266</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
@@ -5722,43 +5928,43 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="G1" s="19"/>
+        <v>272</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
auto:changes in the level of care assessment form
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="291">
   <si>
     <t>type</t>
   </si>
@@ -256,13 +256,28 @@
     <t>h1 yellow</t>
   </si>
   <si>
+    <t xml:space="preserve">person_completing </t>
+  </si>
+  <si>
+    <t>Name of Person Completing form:</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_care_form</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Date of Level of Care Assessment:</t>
+  </si>
+  <si>
     <t>select_one medical</t>
   </si>
   <si>
     <t>medical</t>
   </si>
   <si>
-    <t>Medical care</t>
+    <t>Medical care*</t>
   </si>
   <si>
     <t>select_one knowledge</t>
@@ -416,13 +431,6 @@
     <t xml:space="preserve"> if((${score} &gt;= 1 and ${score} &lt;= 15), 'Limitted', if((${score} &gt;= 16  and ${score} &lt; 40 ), 'Supportive', if((${score} &gt;= 40), 'Comprehensive','')))</t>
   </si>
   <si>
-    <t xml:space="preserve">findings </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Significant Findings 
-</t>
-  </si>
-  <si>
     <t>score_note</t>
   </si>
   <si>
@@ -432,7 +440,7 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">Score is: </t>
+      <t xml:space="preserve">**Score is:** </t>
     </r>
     <r>
       <rPr>
@@ -446,7 +454,7 @@
     <t>category_note</t>
   </si>
   <si>
-    <t>Risk Category is:${category}</t>
+    <t>**Risk Category is:** ${category}</t>
   </si>
   <si>
     <t>note_1</t>
@@ -467,16 +475,28 @@
     <t>40+ Comprehensive 	 Cases reviewed at least twice every month</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>date_assesment</t>
   </si>
   <si>
-    <t xml:space="preserve"> Date of Level of Care Assessment:</t>
-  </si>
-  <si>
     <t>today()</t>
+  </si>
+  <si>
+    <t>select_one refer</t>
+  </si>
+  <si>
+    <t>refer_to</t>
+  </si>
+  <si>
+    <t>Refer to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">findings </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Significant Findings</t>
   </si>
   <si>
     <t>list_name</t>
@@ -895,6 +915,27 @@
   <si>
     <t xml:space="preserve">Major - Major dental needs; needs pay source or denied; noncompliant in correcting issues 
 </t>
+  </si>
+  <si>
+    <t>refer</t>
+  </si>
+  <si>
+    <t>refer_limitted</t>
+  </si>
+  <si>
+    <t>Limited - cases reviewed as needed, but at least annually</t>
+  </si>
+  <si>
+    <t>refer_suppportive</t>
+  </si>
+  <si>
+    <t>Supportive - cases reviewed at least every 6 months</t>
+  </si>
+  <si>
+    <t>refer_comprehensive</t>
+  </si>
+  <si>
+    <t>Comprehensive - Cases reviewed at least twice every month</t>
   </si>
   <si>
     <t>form_title</t>
@@ -931,7 +972,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -987,6 +1028,11 @@
       <sz val="12.0"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1046,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1093,6 +1139,12 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1112,10 +1164,13 @@
     <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -3031,330 +3086,410 @@
       <c r="AA48" s="17"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="15"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="17"/>
+      <c r="Z49" s="17"/>
+      <c r="AA49" s="17"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="18"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="3" t="s">
+      <c r="B50" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="18"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="17"/>
+      <c r="Y50" s="17"/>
+      <c r="Z50" s="17"/>
+      <c r="AA50" s="17"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="D51" s="3"/>
-      <c r="E51" s="18"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="18"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="20"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="3"/>
+      <c r="E53" s="20"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="18"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="12" t="s">
+      <c r="B54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="C54" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="D54" s="3"/>
-      <c r="E54" s="18"/>
+      <c r="E54" s="20"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3"/>
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="18"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="3" t="s">
+      <c r="B56" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D56" s="3"/>
-      <c r="E56" s="18"/>
+      <c r="E56" s="20"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="18"/>
+      <c r="E57" s="20"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="3"/>
+      <c r="E58" s="20"/>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="18"/>
-    </row>
-    <row r="59" ht="18.75" customHeight="1">
-      <c r="A59" s="19" t="s">
+      <c r="B59" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="C59" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="D59" s="3"/>
+      <c r="E59" s="20"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D59" s="19"/>
-      <c r="E59" s="18"/>
-    </row>
-    <row r="60" ht="18.75" customHeight="1">
-      <c r="A60" s="19" t="s">
+      <c r="B60" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="C60" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="D60" s="3"/>
+      <c r="E60" s="20"/>
+    </row>
+    <row r="61" ht="18.75" customHeight="1">
+      <c r="A61" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="19"/>
-      <c r="E60" s="18"/>
-    </row>
-    <row r="61" ht="18.75" customHeight="1">
-      <c r="A61" s="19" t="s">
+      <c r="B61" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="C61" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="D61" s="21"/>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" ht="18.75" customHeight="1">
+      <c r="A62" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="18"/>
-    </row>
-    <row r="62" ht="18.75" customHeight="1">
-      <c r="A62" s="19" t="s">
+      <c r="B62" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="C62" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="D62" s="21"/>
+      <c r="E62" s="20"/>
+    </row>
+    <row r="63" ht="18.75" customHeight="1">
+      <c r="A63" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="19"/>
-      <c r="E62" s="18"/>
-    </row>
-    <row r="63" ht="18.75" customHeight="1">
-      <c r="A63" s="19" t="s">
+      <c r="B63" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="C63" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="D63" s="21"/>
+      <c r="E63" s="20"/>
+    </row>
+    <row r="64" ht="18.75" customHeight="1">
+      <c r="A64" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="18"/>
-    </row>
-    <row r="64" ht="224.25" customHeight="1">
-      <c r="A64" s="19" t="s">
+      <c r="B64" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" ht="18.75" customHeight="1">
+      <c r="A65" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" ht="224.25" customHeight="1">
+      <c r="A66" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="19" t="s">
+      <c r="B66" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B66" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="18"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="19" t="s">
+      <c r="B67" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="18"/>
-    </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="19" t="s">
+      <c r="B68" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="18"/>
+      <c r="C68" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="20"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="18"/>
+      <c r="C69" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="21"/>
+      <c r="E69" s="20"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="21" t="s">
+      <c r="B70" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="18"/>
+      <c r="C70" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="21"/>
+      <c r="E70" s="20"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="21" t="s">
+      <c r="B71" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="18"/>
+      <c r="C71" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="20"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="21" t="s">
+      <c r="A72" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="20" t="s">
+      <c r="D72" s="21"/>
+      <c r="E72" s="20"/>
+    </row>
+    <row r="73" ht="15.75" customHeight="1">
+      <c r="A73" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="23" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="3" t="s">
+      <c r="C73" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="21"/>
+      <c r="E73" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" ht="15.75" customHeight="1">
+      <c r="A74" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D74" s="21"/>
+      <c r="E74" s="22"/>
+    </row>
+    <row r="75" ht="15.75" customHeight="1">
+      <c r="A75" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D75" s="21"/>
+      <c r="E75" s="22"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1">
+      <c r="A76" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="3"/>
+    </row>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1"/>
     <row r="80" ht="15.75" customHeight="1"/>
@@ -4311,9 +4446,12 @@
     <row r="1031" ht="15.75" customHeight="1"/>
     <row r="1032" ht="15.75" customHeight="1"/>
     <row r="1033" ht="15.75" customHeight="1"/>
+    <row r="1034" ht="15.75" customHeight="1"/>
+    <row r="1035" ht="15.75" customHeight="1"/>
+    <row r="1036" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D48">
+    <dataValidation type="list" allowBlank="1" sqref="D48:D50">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4338,679 +4476,709 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="23" t="s">
-        <v>96</v>
+      <c r="A22" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="23" t="s">
-        <v>96</v>
+      <c r="A23" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>190</v>
+        <v>196</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="23" t="s">
-        <v>96</v>
+      <c r="A24" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>192</v>
+        <v>198</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="23" t="s">
-        <v>96</v>
+      <c r="A25" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>194</v>
+        <v>200</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>202</v>
+      <c r="A29" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>209</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" ht="15.75" customHeight="1">
+      <c r="A64" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>280</v>
+      </c>
+    </row>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -5975,28 +6143,28 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>272</v>
-      </c>
-      <c r="G1" s="26"/>
+        <v>285</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>69</v>
@@ -6005,13 +6173,13 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updating the app forms
</commit_message>
<xml_diff>
--- a/config/forms/app/care.xlsx
+++ b/config/forms/app/care.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="280">
   <si>
     <t>type</t>
   </si>
@@ -431,7 +431,7 @@
     <t xml:space="preserve">category </t>
   </si>
   <si>
-    <t xml:space="preserve"> if((${score} &gt;= 1 and ${score} &lt;= 15), 'Limitted', if((${score} &gt;= 16  and ${score} &lt; 40 ), 'Supportive', if((${score} &gt;= 40), 'Comprehensive','')))</t>
+    <t xml:space="preserve"> if((${score} &gt;= 1 and ${score} &lt;= 15), 'Limited', if((${score} &gt;= 16  and ${score} &lt; 40 ), 'Supportive', if((${score} &gt;= 40), 'Comprehensive','')))</t>
   </si>
   <si>
     <t>score_note</t>
@@ -478,21 +478,6 @@
     <t>40+ Comprehensive 	 Cases reviewed at least twice every month</t>
   </si>
   <si>
-    <t>date_assesment</t>
-  </si>
-  <si>
-    <t>today()</t>
-  </si>
-  <si>
-    <t>select_one refer</t>
-  </si>
-  <si>
-    <t>refer_to</t>
-  </si>
-  <si>
-    <t>Refer to</t>
-  </si>
-  <si>
     <t xml:space="preserve">string </t>
   </si>
   <si>
@@ -918,27 +903,6 @@
   <si>
     <t xml:space="preserve">Major - Major dental needs; needs pay source or denied; noncompliant in correcting issues 
 </t>
-  </si>
-  <si>
-    <t>refer</t>
-  </si>
-  <si>
-    <t>refer_limitted</t>
-  </si>
-  <si>
-    <t>Limited - cases reviewed as needed, but at least annually</t>
-  </si>
-  <si>
-    <t>refer_suppportive</t>
-  </si>
-  <si>
-    <t>Supportive - cases reviewed at least every 6 months</t>
-  </si>
-  <si>
-    <t>refer_comprehensive</t>
-  </si>
-  <si>
-    <t>Comprehensive - Cases reviewed at least twice every month</t>
   </si>
   <si>
     <t>form_title</t>
@@ -975,7 +939,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1038,11 +1002,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1100,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1181,13 +1140,10 @@
     <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -3492,7 +3448,7 @@
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
       <c r="E67" s="24"/>
-      <c r="F67" s="23" t="s">
+      <c r="F67" s="25" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3568,56 +3524,28 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="26" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="D73" s="26"/>
       <c r="E73" s="24"/>
-      <c r="F73" s="25" t="s">
-        <v>146</v>
-      </c>
+      <c r="F73" s="25"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B74" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" s="26"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="25"/>
+      <c r="A74" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B75" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C75" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D75" s="26"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="25"/>
-    </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="4"/>
-    </row>
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
     <row r="78" ht="15.75" customHeight="1"/>
     <row r="79" ht="15.75" customHeight="1"/>
     <row r="80" ht="15.75" customHeight="1"/>
@@ -4575,8 +4503,6 @@
     <row r="1032" ht="15.75" customHeight="1"/>
     <row r="1033" ht="15.75" customHeight="1"/>
     <row r="1034" ht="15.75" customHeight="1"/>
-    <row r="1035" ht="15.75" customHeight="1"/>
-    <row r="1036" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="E48:E50">
@@ -4605,7 +4531,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>1</v>
@@ -4619,10 +4545,10 @@
         <v>87</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -4630,10 +4556,10 @@
         <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -4641,10 +4567,10 @@
         <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -4652,10 +4578,10 @@
         <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -4663,10 +4589,10 @@
         <v>90</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -4674,10 +4600,10 @@
         <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -4685,10 +4611,10 @@
         <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -4696,10 +4622,10 @@
         <v>90</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -4707,10 +4633,10 @@
         <v>93</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -4718,10 +4644,10 @@
         <v>93</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -4729,10 +4655,10 @@
         <v>93</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -4740,54 +4666,54 @@
         <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="C16" s="15" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -4795,10 +4721,10 @@
         <v>99</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -4806,10 +4732,10 @@
         <v>99</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -4817,10 +4743,10 @@
         <v>99</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -4828,10 +4754,10 @@
         <v>99</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -4839,10 +4765,10 @@
         <v>102</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -4850,10 +4776,10 @@
         <v>102</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -4861,10 +4787,10 @@
         <v>102</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -4872,10 +4798,10 @@
         <v>102</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -4883,10 +4809,10 @@
         <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -4894,10 +4820,10 @@
         <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -4905,21 +4831,21 @@
         <v>105</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="28" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -4927,10 +4853,10 @@
         <v>108</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -4938,10 +4864,10 @@
         <v>108</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -4949,10 +4875,10 @@
         <v>108</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -4960,10 +4886,10 @@
         <v>108</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -4971,10 +4897,10 @@
         <v>111</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -4982,10 +4908,10 @@
         <v>111</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -4993,10 +4919,10 @@
         <v>111</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -5004,10 +4930,10 @@
         <v>111</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -5015,10 +4941,10 @@
         <v>114</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -5026,10 +4952,10 @@
         <v>114</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -5037,10 +4963,10 @@
         <v>114</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -5048,10 +4974,10 @@
         <v>114</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -5059,10 +4985,10 @@
         <v>117</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -5070,10 +4996,10 @@
         <v>117</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -5081,10 +5007,10 @@
         <v>117</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -5092,10 +5018,10 @@
         <v>117</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -5103,10 +5029,10 @@
         <v>120</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -5114,10 +5040,10 @@
         <v>120</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -5125,10 +5051,10 @@
         <v>120</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -5136,10 +5062,10 @@
         <v>120</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -5147,10 +5073,10 @@
         <v>123</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -5158,10 +5084,10 @@
         <v>123</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -5169,10 +5095,10 @@
         <v>123</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -5180,10 +5106,10 @@
         <v>123</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -5191,10 +5117,10 @@
         <v>126</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -5202,10 +5128,10 @@
         <v>126</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -5213,10 +5139,10 @@
         <v>126</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -5224,10 +5150,10 @@
         <v>126</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -5235,10 +5161,10 @@
         <v>129</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -5246,10 +5172,10 @@
         <v>129</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -5257,10 +5183,10 @@
         <v>129</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -5268,45 +5194,15 @@
         <v>129</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="B64" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="C64" s="30" t="s">
-        <v>281</v>
-      </c>
-    </row>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -6271,28 +6167,28 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>287</v>
-      </c>
-      <c r="G1" s="32"/>
+        <v>274</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>70</v>
@@ -6301,13 +6197,13 @@
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>

</xml_diff>